<commit_message>
update files on global-requirements
</commit_message>
<xml_diff>
--- a/25.1.Epoxy/dependencies.xlsx
+++ b/25.1.Epoxy/dependencies.xlsx
@@ -1864,8 +1864,8 @@
   </sheetPr>
   <dimension ref="A1:XFD733"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A601" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A599" activeCellId="0" sqref="599:599"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A691" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A711" activeCellId="0" sqref="711:711"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32150,29 +32150,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="711" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B711" s="1" t="s">
+    <row r="711" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B711" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="C711" s="1" t="s">
+      <c r="C711" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="D711" s="1" t="s">
+      <c r="D711" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="E711" s="2" t="s">
+      <c r="E711" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F711" s="9" t="s">
+      <c r="F711" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="G711" s="9" t="s">
+      <c r="G711" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J711" s="1" t="s">
+      <c r="H711" s="16"/>
+      <c r="I711" s="16"/>
+      <c r="J711" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="K711" s="1" t="s">
+      <c r="K711" s="15" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update oslo.db & deps
</commit_message>
<xml_diff>
--- a/25.1.Epoxy/dependencies.xlsx
+++ b/25.1.Epoxy/dependencies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3992" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3993" uniqueCount="618">
   <si>
     <t xml:space="preserve">Pkg</t>
   </si>
@@ -1180,7 +1180,7 @@
     <t xml:space="preserve"> typing-extensions&gt;=4</t>
   </si>
   <si>
-    <t xml:space="preserve">i4.1.35</t>
+    <t xml:space="preserve">i4.2.35</t>
   </si>
   <si>
     <t xml:space="preserve">oslo.db</t>
@@ -1634,9 +1634,6 @@
   </si>
   <si>
     <t xml:space="preserve">pbr&gt;=1.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i4.2.35</t>
   </si>
   <si>
     <t xml:space="preserve">i1.2.03</t>
@@ -2351,8 +2348,8 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A716" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A744" activeCellId="0" sqref="744:744"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A985" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1007" activeCellId="0" sqref="B1007"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7900,17 +7897,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B306" s="1" t="s">
+    <row r="306" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B306" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="C306" s="1" t="s">
+      <c r="C306" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="D306" s="1" t="s">
+      <c r="D306" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="E306" s="2" t="s">
+      <c r="E306" s="16" t="s">
         <v>293</v>
       </c>
       <c r="F306" s="16" t="s">
@@ -7919,10 +7916,12 @@
       <c r="G306" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J306" s="1" t="s">
+      <c r="H306" s="16"/>
+      <c r="I306" s="16"/>
+      <c r="J306" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="K306" s="1" t="s">
+      <c r="K306" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -16337,20 +16336,20 @@
       <c r="N728" s="1"/>
       <c r="O728" s="1"/>
     </row>
-    <row r="729" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A729" s="1" t="s">
+    <row r="729" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A729" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B729" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="C729" s="1" t="s">
+      <c r="B729" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="C729" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="D729" s="1" t="s">
+      <c r="D729" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="E729" s="2" t="s">
+      <c r="E729" s="16" t="s">
         <v>293</v>
       </c>
       <c r="F729" s="16" t="s">
@@ -16359,10 +16358,12 @@
       <c r="G729" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J729" s="1" t="s">
+      <c r="H729" s="16"/>
+      <c r="I729" s="16"/>
+      <c r="J729" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="K729" s="1" t="s">
+      <c r="K729" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -16388,16 +16389,16 @@
         <v>5</v>
       </c>
       <c r="B731" s="15" t="s">
+        <v>538</v>
+      </c>
+      <c r="C731" s="15" t="s">
         <v>539</v>
       </c>
-      <c r="C731" s="15" t="s">
+      <c r="D731" s="15" t="s">
         <v>540</v>
       </c>
-      <c r="D731" s="15" t="s">
+      <c r="E731" s="16" t="s">
         <v>541</v>
-      </c>
-      <c r="E731" s="16" t="s">
-        <v>542</v>
       </c>
       <c r="F731" s="16" t="s">
         <v>9</v>
@@ -16410,7 +16411,7 @@
       </c>
       <c r="I731" s="16"/>
       <c r="J731" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="732" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16439,7 +16440,7 @@
       <c r="H733" s="9"/>
       <c r="I733" s="9"/>
       <c r="J733" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="734" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16450,16 +16451,16 @@
     </row>
     <row r="736" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B736" s="15" t="s">
+        <v>544</v>
+      </c>
+      <c r="C736" s="15" t="s">
         <v>545</v>
       </c>
-      <c r="C736" s="15" t="s">
+      <c r="D736" s="15" t="s">
         <v>546</v>
       </c>
-      <c r="D736" s="15" t="s">
+      <c r="E736" s="16" t="s">
         <v>547</v>
-      </c>
-      <c r="E736" s="16" t="s">
-        <v>548</v>
       </c>
       <c r="F736" s="16" t="s">
         <v>9</v>
@@ -16470,7 +16471,7 @@
       <c r="H736" s="16"/>
       <c r="I736" s="16"/>
       <c r="J736" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="737" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16514,16 +16515,16 @@
         <v>5</v>
       </c>
       <c r="B739" s="15" t="s">
+        <v>544</v>
+      </c>
+      <c r="C739" s="15" t="s">
         <v>545</v>
       </c>
-      <c r="C739" s="15" t="s">
+      <c r="D739" s="15" t="s">
         <v>546</v>
       </c>
-      <c r="D739" s="15" t="s">
+      <c r="E739" s="16" t="s">
         <v>547</v>
-      </c>
-      <c r="E739" s="16" t="s">
-        <v>548</v>
       </c>
       <c r="F739" s="16" t="s">
         <v>9</v>
@@ -16536,7 +16537,7 @@
       </c>
       <c r="I739" s="16"/>
       <c r="J739" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="740" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16547,16 +16548,16 @@
     </row>
     <row r="742" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B742" s="15" t="s">
+        <v>538</v>
+      </c>
+      <c r="C742" s="15" t="s">
         <v>539</v>
       </c>
-      <c r="C742" s="15" t="s">
+      <c r="D742" s="15" t="s">
         <v>540</v>
       </c>
-      <c r="D742" s="15" t="s">
+      <c r="E742" s="16" t="s">
         <v>541</v>
-      </c>
-      <c r="E742" s="16" t="s">
-        <v>542</v>
       </c>
       <c r="F742" s="16" t="s">
         <v>9</v>
@@ -16567,7 +16568,7 @@
       <c r="H742" s="16"/>
       <c r="I742" s="16"/>
       <c r="J742" s="15" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="743" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16576,16 +16577,16 @@
         <v>13</v>
       </c>
       <c r="B744" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="C744" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="C744" s="15" t="s">
+      <c r="D744" s="15" t="s">
         <v>550</v>
       </c>
-      <c r="D744" s="15" t="s">
+      <c r="E744" s="16" t="s">
         <v>551</v>
-      </c>
-      <c r="E744" s="16" t="s">
-        <v>552</v>
       </c>
       <c r="F744" s="16" t="s">
         <v>9</v>
@@ -16596,7 +16597,7 @@
       <c r="H744" s="16"/>
       <c r="I744" s="16"/>
       <c r="J744" s="15" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K744" s="15" t="s">
         <v>536</v>
@@ -16624,16 +16625,16 @@
         <v>5</v>
       </c>
       <c r="B746" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="C746" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="C746" s="15" t="s">
+      <c r="D746" s="15" t="s">
         <v>550</v>
       </c>
-      <c r="D746" s="15" t="s">
+      <c r="E746" s="16" t="s">
         <v>551</v>
-      </c>
-      <c r="E746" s="16" t="s">
-        <v>552</v>
       </c>
       <c r="F746" s="16" t="s">
         <v>9</v>
@@ -16646,7 +16647,7 @@
       </c>
       <c r="I746" s="16"/>
       <c r="J746" s="15" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K746" s="15" t="s">
         <v>536</v>
@@ -16710,21 +16711,21 @@
       <c r="H749" s="9"/>
       <c r="I749" s="9"/>
       <c r="J749" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="750" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B750" s="15" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C750" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="D750" s="15" t="s">
         <v>546</v>
       </c>
-      <c r="D750" s="15" t="s">
+      <c r="E750" s="16" t="s">
         <v>547</v>
-      </c>
-      <c r="E750" s="16" t="s">
-        <v>548</v>
       </c>
       <c r="F750" s="16" t="s">
         <v>9</v>
@@ -16735,7 +16736,7 @@
       <c r="H750" s="16"/>
       <c r="I750" s="16"/>
       <c r="J750" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="751" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16755,20 +16756,20 @@
       <c r="N751" s="1"/>
       <c r="O751" s="1"/>
     </row>
-    <row r="752" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A752" s="1" t="s">
+    <row r="752" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A752" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B752" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="C752" s="1" t="s">
+      <c r="B752" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="C752" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="D752" s="1" t="s">
+      <c r="D752" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="E752" s="2" t="s">
+      <c r="E752" s="16" t="s">
         <v>293</v>
       </c>
       <c r="F752" s="16" t="s">
@@ -16777,10 +16778,12 @@
       <c r="G752" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J752" s="1" t="s">
+      <c r="H752" s="16"/>
+      <c r="I752" s="16"/>
+      <c r="J752" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="K752" s="1" t="s">
+      <c r="K752" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -16957,16 +16960,16 @@
         <v>5</v>
       </c>
       <c r="B763" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="C763" s="15" t="s">
         <v>556</v>
-      </c>
-      <c r="C763" s="15" t="s">
-        <v>557</v>
       </c>
       <c r="D763" s="15" t="s">
         <v>276</v>
       </c>
       <c r="E763" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F763" s="16" t="s">
         <v>154</v>
@@ -16979,7 +16982,7 @@
       </c>
       <c r="I763" s="16"/>
       <c r="J763" s="15" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="K763" s="15" t="s">
         <v>42</v>
@@ -17151,7 +17154,7 @@
       <c r="H771" s="2"/>
       <c r="I771" s="2"/>
       <c r="J771" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="K771" s="1" t="s">
         <v>42</v>
@@ -17432,7 +17435,7 @@
     </row>
     <row r="787" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B787" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D787" s="3" t="s">
         <v>527</v>
@@ -17749,7 +17752,7 @@
       <c r="H799" s="9"/>
       <c r="I799" s="9"/>
       <c r="J799" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="K799" s="7" t="s">
         <v>42</v>
@@ -17923,7 +17926,7 @@
       <c r="H805" s="9"/>
       <c r="I805" s="9"/>
       <c r="J805" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K805" s="7" t="s">
         <v>128</v>
@@ -18247,7 +18250,7 @@
       <c r="H821" s="9"/>
       <c r="I821" s="9"/>
       <c r="J821" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K821" s="7" t="s">
         <v>42</v>
@@ -18275,7 +18278,7 @@
       <c r="H822" s="9"/>
       <c r="I822" s="9"/>
       <c r="J822" s="7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K822" s="7" t="s">
         <v>42</v>
@@ -18762,7 +18765,7 @@
       <c r="H845" s="9"/>
       <c r="I845" s="9"/>
       <c r="J845" s="7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="K845" s="7" t="s">
         <v>75</v>
@@ -18790,7 +18793,7 @@
       <c r="H846" s="9"/>
       <c r="I846" s="9"/>
       <c r="J846" s="7" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="K846" s="7" t="s">
         <v>42</v>
@@ -18818,7 +18821,7 @@
       <c r="H847" s="9"/>
       <c r="I847" s="9"/>
       <c r="J847" s="7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="K847" s="7" t="s">
         <v>42</v>
@@ -18874,7 +18877,7 @@
       <c r="H849" s="9"/>
       <c r="I849" s="9"/>
       <c r="J849" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="K849" s="7" t="s">
         <v>42</v>
@@ -18973,20 +18976,20 @@
       <c r="N853" s="10"/>
       <c r="O853" s="10"/>
     </row>
-    <row r="854" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A854" s="1" t="s">
+    <row r="854" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A854" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B854" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="C854" s="1" t="s">
+      <c r="B854" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="C854" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="D854" s="1" t="s">
+      <c r="D854" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="E854" s="2" t="s">
+      <c r="E854" s="16" t="s">
         <v>293</v>
       </c>
       <c r="F854" s="16" t="s">
@@ -18995,10 +18998,14 @@
       <c r="G854" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J854" s="1" t="s">
+      <c r="H854" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I854" s="16"/>
+      <c r="J854" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="K854" s="1" t="s">
+      <c r="K854" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -19319,7 +19326,7 @@
       <c r="H868" s="2"/>
       <c r="I868" s="2"/>
       <c r="J868" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K868" s="1"/>
       <c r="L868" s="1"/>
@@ -19338,7 +19345,7 @@
       <c r="H869" s="2"/>
       <c r="I869" s="2"/>
       <c r="J869" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="K869" s="1"/>
       <c r="L869" s="1"/>
@@ -19346,77 +19353,67 @@
       <c r="N869" s="1"/>
       <c r="O869" s="1"/>
       <c r="T869" s="13" t="s">
+        <v>571</v>
+      </c>
+      <c r="U869" s="13" t="s">
         <v>572</v>
       </c>
-      <c r="U869" s="13" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="870" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A870" s="1"/>
-      <c r="B870" s="1" t="s">
+    </row>
+    <row r="870" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B870" s="15" t="s">
         <v>531</v>
       </c>
-      <c r="C870" s="1" t="s">
+      <c r="C870" s="15" t="s">
         <v>532</v>
       </c>
-      <c r="D870" s="1" t="s">
+      <c r="D870" s="15" t="s">
         <v>533</v>
       </c>
-      <c r="E870" s="2" t="s">
+      <c r="E870" s="16" t="s">
         <v>534</v>
       </c>
-      <c r="F870" s="2" t="s">
+      <c r="F870" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G870" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H870" s="2"/>
-      <c r="I870" s="2"/>
-      <c r="J870" s="1" t="s">
+      <c r="G870" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H870" s="16"/>
+      <c r="I870" s="16"/>
+      <c r="J870" s="15" t="s">
         <v>535</v>
       </c>
-      <c r="K870" s="1" t="s">
+      <c r="K870" s="15" t="s">
         <v>536</v>
       </c>
-      <c r="L870" s="1"/>
-      <c r="M870" s="1"/>
-      <c r="N870" s="1"/>
-      <c r="O870" s="1"/>
-    </row>
-    <row r="871" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A871" s="1"/>
-      <c r="B871" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="C871" s="1" t="s">
+    </row>
+    <row r="871" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B871" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="C871" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="D871" s="15" t="s">
         <v>550</v>
       </c>
-      <c r="D871" s="1" t="s">
+      <c r="E871" s="16" t="s">
         <v>551</v>
       </c>
-      <c r="E871" s="2" t="s">
+      <c r="F871" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G871" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H871" s="16"/>
+      <c r="I871" s="16"/>
+      <c r="J871" s="15" t="s">
         <v>552</v>
       </c>
-      <c r="F871" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G871" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H871" s="2"/>
-      <c r="I871" s="2"/>
-      <c r="J871" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="K871" s="1" t="s">
+      <c r="K871" s="15" t="s">
         <v>536</v>
       </c>
-      <c r="L871" s="1"/>
-      <c r="M871" s="1"/>
-      <c r="N871" s="1"/>
-      <c r="O871" s="1"/>
     </row>
     <row r="872" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A872" s="1"/>
@@ -19845,7 +19842,7 @@
       <c r="H894" s="9"/>
       <c r="I894" s="9"/>
       <c r="J894" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="K894" s="7" t="s">
         <v>42</v>
@@ -20077,16 +20074,16 @@
     </row>
     <row r="903" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B903" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="C903" s="15" t="s">
         <v>556</v>
-      </c>
-      <c r="C903" s="15" t="s">
-        <v>557</v>
       </c>
       <c r="D903" s="15" t="s">
         <v>276</v>
       </c>
       <c r="E903" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F903" s="16" t="s">
         <v>154</v>
@@ -20097,7 +20094,7 @@
       <c r="H903" s="16"/>
       <c r="I903" s="16"/>
       <c r="J903" s="15" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="K903" s="15" t="s">
         <v>42</v>
@@ -20153,7 +20150,7 @@
       <c r="H905" s="9"/>
       <c r="I905" s="9"/>
       <c r="J905" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="K905" s="7" t="s">
         <v>42</v>
@@ -20505,7 +20502,7 @@
       <c r="H922" s="9"/>
       <c r="I922" s="9"/>
       <c r="J922" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="K922" s="7" t="s">
         <v>42</v>
@@ -20561,7 +20558,7 @@
       <c r="H924" s="9"/>
       <c r="I924" s="9"/>
       <c r="J924" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K924" s="7" t="s">
         <v>42</v>
@@ -20589,7 +20586,7 @@
       <c r="H925" s="9"/>
       <c r="I925" s="9"/>
       <c r="J925" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K925" s="7" t="s">
         <v>42</v>
@@ -20617,7 +20614,7 @@
       <c r="H926" s="9"/>
       <c r="I926" s="9"/>
       <c r="J926" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K926" s="7" t="s">
         <v>42</v>
@@ -20645,7 +20642,7 @@
       <c r="H927" s="9"/>
       <c r="I927" s="9"/>
       <c r="J927" s="7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="K927" s="7" t="s">
         <v>42</v>
@@ -20673,7 +20670,7 @@
       <c r="H928" s="9"/>
       <c r="I928" s="9"/>
       <c r="J928" s="7" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K928" s="7" t="s">
         <v>42</v>
@@ -20826,25 +20823,25 @@
       <c r="N935" s="1"/>
       <c r="O935" s="1"/>
       <c r="R935" s="13" t="s">
+        <v>581</v>
+      </c>
+      <c r="S935" s="13" t="s">
         <v>582</v>
       </c>
-      <c r="S935" s="13" t="s">
+      <c r="T935" s="13" t="s">
         <v>583</v>
       </c>
-      <c r="T935" s="13" t="s">
+      <c r="U935" s="13" t="s">
         <v>584</v>
       </c>
-      <c r="U935" s="13" t="s">
+      <c r="V935" s="13" t="s">
         <v>585</v>
       </c>
-      <c r="V935" s="13" t="s">
+      <c r="W935" s="13" t="s">
         <v>586</v>
       </c>
-      <c r="W935" s="13" t="s">
-        <v>587</v>
-      </c>
       <c r="X935" s="13" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="936" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20866,31 +20863,31 @@
       <c r="N936" s="1"/>
       <c r="O936" s="1"/>
       <c r="R936" s="13" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="S936" s="13" t="s">
         <v>58</v>
       </c>
       <c r="T936" s="13" t="s">
+        <v>588</v>
+      </c>
+      <c r="U936" s="13" t="s">
         <v>589</v>
       </c>
-      <c r="U936" s="13" t="s">
+      <c r="V936" s="13" t="s">
         <v>590</v>
       </c>
-      <c r="V936" s="13" t="s">
+      <c r="W936" s="13" t="s">
+        <v>585</v>
+      </c>
+      <c r="X936" s="13" t="s">
         <v>591</v>
       </c>
-      <c r="W936" s="13" t="s">
-        <v>586</v>
-      </c>
-      <c r="X936" s="13" t="s">
+      <c r="Y936" s="13" t="s">
         <v>592</v>
       </c>
-      <c r="Y936" s="13" t="s">
+      <c r="Z936" s="13" t="s">
         <v>593</v>
-      </c>
-      <c r="Z936" s="13" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="937" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20912,22 +20909,22 @@
       <c r="N937" s="1"/>
       <c r="O937" s="1"/>
       <c r="R937" s="13" t="s">
+        <v>594</v>
+      </c>
+      <c r="S937" s="13" t="s">
         <v>595</v>
       </c>
-      <c r="S937" s="13" t="s">
+      <c r="T937" s="13" t="s">
         <v>596</v>
       </c>
-      <c r="T937" s="13" t="s">
+      <c r="U937" s="13" t="s">
         <v>597</v>
       </c>
-      <c r="U937" s="13" t="s">
+      <c r="V937" s="13" t="s">
         <v>598</v>
       </c>
-      <c r="V937" s="13" t="s">
+      <c r="W937" s="13" t="s">
         <v>599</v>
-      </c>
-      <c r="W937" s="13" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="938" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21025,7 +21022,7 @@
       <c r="H941" s="9"/>
       <c r="I941" s="9"/>
       <c r="J941" s="7" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="K941" s="7" t="s">
         <v>42</v>
@@ -21339,7 +21336,7 @@
     </row>
     <row r="955" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B955" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E955" s="4"/>
       <c r="F955" s="4" t="s">
@@ -21592,7 +21589,7 @@
         <v>412</v>
       </c>
       <c r="C971" s="7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D971" s="7" t="s">
         <v>414</v>
@@ -21693,7 +21690,7 @@
       <c r="H974" s="9"/>
       <c r="I974" s="9"/>
       <c r="J974" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="K974" s="7" t="s">
         <v>42</v>
@@ -38104,7 +38101,7 @@
     </row>
     <row r="978" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B978" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E978" s="4"/>
       <c r="F978" s="4" t="s">
@@ -38407,7 +38404,7 @@
       <c r="H998" s="9"/>
       <c r="I998" s="9"/>
       <c r="J998" s="7" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="K998" s="7" t="s">
         <v>42</v>
@@ -38547,7 +38544,7 @@
       <c r="H1003" s="9"/>
       <c r="I1003" s="9"/>
       <c r="J1003" s="7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="K1003" s="7" t="s">
         <v>42</v>
@@ -38575,7 +38572,7 @@
       <c r="H1004" s="16"/>
       <c r="I1004" s="16"/>
       <c r="J1004" s="15" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="K1004" s="15" t="s">
         <v>42</v>
@@ -38609,17 +38606,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="1006" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1006" s="1" t="s">
+    <row r="1006" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1006" s="15" t="s">
         <v>386</v>
       </c>
-      <c r="C1006" s="1" t="s">
+      <c r="C1006" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="D1006" s="1" t="s">
+      <c r="D1006" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="E1006" s="2" t="s">
+      <c r="E1006" s="16" t="s">
         <v>293</v>
       </c>
       <c r="F1006" s="16" t="s">
@@ -38628,10 +38625,12 @@
       <c r="G1006" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J1006" s="1" t="s">
+      <c r="H1006" s="16"/>
+      <c r="I1006" s="16"/>
+      <c r="J1006" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="K1006" s="1" t="s">
+      <c r="K1006" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -38721,7 +38720,7 @@
     </row>
     <row r="1010" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J1010" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="K1010" s="1" t="s">
         <v>42</v>
@@ -38749,7 +38748,7 @@
       <c r="H1011" s="9"/>
       <c r="I1011" s="9"/>
       <c r="J1011" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="K1011" s="7" t="s">
         <v>42</v>
@@ -38757,7 +38756,7 @@
     </row>
     <row r="1012" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J1012" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="K1012" s="1" t="s">
         <v>42</v>
@@ -38793,7 +38792,7 @@
     </row>
     <row r="1014" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J1014" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="K1014" s="1" t="s">
         <v>75</v>
@@ -38801,7 +38800,7 @@
     </row>
     <row r="1015" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J1015" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="1016" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38826,7 +38825,7 @@
       <c r="H1016" s="16"/>
       <c r="I1016" s="16"/>
       <c r="J1016" s="15" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="K1016" s="15" t="s">
         <v>65</v>
@@ -38854,7 +38853,7 @@
       <c r="H1017" s="9"/>
       <c r="I1017" s="9"/>
       <c r="J1017" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="K1017" s="7" t="s">
         <v>75</v>
@@ -38862,7 +38861,7 @@
     </row>
     <row r="1018" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J1018" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="K1018" s="1" t="s">
         <v>65</v>
@@ -38870,16 +38869,16 @@
     </row>
     <row r="1019" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1019" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="C1019" s="15" t="s">
         <v>556</v>
-      </c>
-      <c r="C1019" s="15" t="s">
-        <v>557</v>
       </c>
       <c r="D1019" s="15" t="s">
         <v>276</v>
       </c>
       <c r="E1019" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F1019" s="16" t="s">
         <v>154</v>
@@ -38890,7 +38889,7 @@
       <c r="H1019" s="16"/>
       <c r="I1019" s="16"/>
       <c r="J1019" s="15" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="K1019" s="15" t="s">
         <v>42</v>
@@ -38918,7 +38917,7 @@
       <c r="H1020" s="9"/>
       <c r="I1020" s="9"/>
       <c r="J1020" s="7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="K1020" s="7" t="s">
         <v>42</v>
@@ -38926,7 +38925,7 @@
     </row>
     <row r="1021" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="J1021" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="K1021" s="1" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
fix sequence in I4
</commit_message>
<xml_diff>
--- a/25.1.Epoxy/dependencies.xlsx
+++ b/25.1.Epoxy/dependencies.xlsx
@@ -1690,6 +1690,57 @@
     <t xml:space="preserve">pbr&gt;=3.1.1</t>
   </si>
   <si>
+    <t xml:space="preserve"># General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oslo.utils&gt;=3.41.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oslo.log&gt;=3.44.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oslo.config&gt;=6.9.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Metrics Exporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prometheus-client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jinja2&gt;=2.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSD License (3 clause)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oslo.context&gt;=2.19.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebOb&gt;=1.8.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># NOTE(harlowja): Because oslo.serialization is used by the client libraries,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># adding a new feature to oslo.serialization means adding a new dependency,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b30.13.25.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Msgpack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025/Jun/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msgpack&gt;=0.5.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">oslo.i18n&gt;=3.20.0</t>
   </si>
   <si>
@@ -1712,57 +1763,6 @@
   </si>
   <si>
     <t xml:space="preserve">oslo.cache&gt;=1.26.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oslo.utils&gt;=3.41.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oslo.log&gt;=3.44.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oslo.config&gt;=6.9.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Metrics Exporter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prometheus-client</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jinja2&gt;=2.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSD License (3 clause)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oslo.context&gt;=2.19.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WebOb&gt;=1.8.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># NOTE(harlowja): Because oslo.serialization is used by the client libraries,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># adding a new feature to oslo.serialization means adding a new dependency,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b30.13.25.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Msgpack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025/Jun/13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">msgpack&gt;=0.5.2</t>
   </si>
   <si>
     <t xml:space="preserve">i4.1.42</t>
@@ -2558,8 +2558,8 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A583" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A591" activeCellId="0" sqref="591:591"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A691" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A716" activeCellId="0" sqref="A716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14200,36 +14200,36 @@
       <c r="N620" s="10"/>
       <c r="O620" s="10"/>
     </row>
-    <row r="621" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A621" s="13" t="s">
+    <row r="621" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A621" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B621" s="13" t="s">
+      <c r="B621" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="C621" s="13" t="s">
+      <c r="C621" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="D621" s="13" t="s">
+      <c r="D621" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="E621" s="14" t="s">
+      <c r="E621" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F621" s="14" t="s">
+      <c r="F621" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G621" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H621" s="14" t="s">
+      <c r="G621" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H621" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I621" s="14"/>
-      <c r="J621" s="13" t="s">
+      <c r="I621" s="9"/>
+      <c r="J621" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="K621" s="13" t="s">
+      <c r="K621" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -14616,13 +14616,13 @@
         <v>5</v>
       </c>
       <c r="B639" s="13" t="s">
-        <v>283</v>
+        <v>389</v>
       </c>
       <c r="C639" s="13" t="s">
-        <v>284</v>
+        <v>390</v>
       </c>
       <c r="D639" s="13" t="s">
-        <v>285</v>
+        <v>391</v>
       </c>
       <c r="E639" s="14" t="s">
         <v>97</v>
@@ -14634,11 +14634,11 @@
         <v>10</v>
       </c>
       <c r="H639" s="14" t="s">
-        <v>138</v>
+        <v>70</v>
       </c>
       <c r="I639" s="14"/>
       <c r="J639" s="13" t="s">
-        <v>286</v>
+        <v>392</v>
       </c>
       <c r="K639" s="13" t="s">
         <v>43</v>
@@ -14754,7 +14754,8 @@
       <c r="N645" s="1"/>
       <c r="O645" s="1"/>
     </row>
-    <row r="646" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="646" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A646" s="1"/>
       <c r="B646" s="7" t="s">
         <v>462</v>
       </c>
@@ -14773,80 +14774,65 @@
       <c r="G646" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H646" s="9"/>
-      <c r="I646" s="9"/>
-      <c r="J646" s="7" t="s">
+      <c r="H646" s="2"/>
+      <c r="I646" s="2"/>
+      <c r="J646" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="K646" s="7" t="s">
+      <c r="K646" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="647" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B647" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C647" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D647" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E647" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F647" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G647" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H647" s="9"/>
-      <c r="I647" s="9"/>
-      <c r="J647" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="K647" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="648" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B648" s="7" t="s">
-        <v>529</v>
-      </c>
-      <c r="C648" s="7" t="s">
-        <v>530</v>
-      </c>
-      <c r="D648" s="7" t="s">
-        <v>531</v>
-      </c>
-      <c r="E648" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F648" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G648" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H648" s="9"/>
-      <c r="I648" s="9"/>
-      <c r="J648" s="7" t="s">
-        <v>532</v>
-      </c>
-      <c r="K648" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="649" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L646" s="1"/>
+      <c r="M646" s="1"/>
+      <c r="N646" s="1"/>
+      <c r="O646" s="1"/>
+    </row>
+    <row r="647" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A647" s="1"/>
+      <c r="B647" s="1"/>
+      <c r="C647" s="1"/>
+      <c r="D647" s="1"/>
+      <c r="E647" s="2"/>
+      <c r="F647" s="2"/>
+      <c r="G647" s="2"/>
+      <c r="H647" s="2"/>
+      <c r="I647" s="2"/>
+      <c r="J647" s="1"/>
+      <c r="K647" s="1"/>
+      <c r="L647" s="1"/>
+      <c r="M647" s="1"/>
+      <c r="N647" s="1"/>
+      <c r="O647" s="1"/>
+    </row>
+    <row r="648" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A648" s="1"/>
+      <c r="B648" s="1"/>
+      <c r="C648" s="1"/>
+      <c r="D648" s="1"/>
+      <c r="E648" s="2"/>
+      <c r="F648" s="2"/>
+      <c r="G648" s="2"/>
+      <c r="H648" s="2"/>
+      <c r="I648" s="2"/>
+      <c r="J648" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="K648" s="1"/>
+      <c r="L648" s="1"/>
+      <c r="M648" s="1"/>
+      <c r="N648" s="1"/>
+      <c r="O648" s="1"/>
+    </row>
+    <row r="649" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A649" s="1"/>
       <c r="B649" s="7" t="s">
-        <v>482</v>
+        <v>114</v>
       </c>
       <c r="C649" s="7" t="s">
-        <v>483</v>
+        <v>115</v>
       </c>
       <c r="D649" s="7" t="s">
-        <v>484</v>
+        <v>116</v>
       </c>
       <c r="E649" s="9" t="s">
         <v>97</v>
@@ -14857,52 +14843,58 @@
       <c r="G649" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H649" s="9"/>
-      <c r="I649" s="9"/>
-      <c r="J649" s="7" t="s">
-        <v>556</v>
-      </c>
-      <c r="K649" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="650" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B650" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C650" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D650" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E650" s="9" t="s">
+      <c r="H649" s="2"/>
+      <c r="I649" s="2"/>
+      <c r="J649" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="K649" s="1"/>
+      <c r="L649" s="1"/>
+      <c r="M649" s="1"/>
+      <c r="N649" s="1"/>
+      <c r="O649" s="1"/>
+    </row>
+    <row r="650" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A650" s="1"/>
+      <c r="B650" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C650" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D650" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="E650" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F650" s="9" t="s">
+      <c r="F650" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G650" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H650" s="9"/>
-      <c r="I650" s="9"/>
-      <c r="J650" s="7" t="s">
-        <v>557</v>
-      </c>
-      <c r="K650" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="651" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G650" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H650" s="2"/>
+      <c r="I650" s="2"/>
+      <c r="J650" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="K650" s="1"/>
+      <c r="L650" s="1"/>
+      <c r="M650" s="1"/>
+      <c r="N650" s="1"/>
+      <c r="O650" s="1"/>
+    </row>
+    <row r="651" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A651" s="1"/>
       <c r="B651" s="7" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="C651" s="7" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="D651" s="7" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="E651" s="9" t="s">
         <v>97</v>
@@ -14913,190 +14905,178 @@
       <c r="G651" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H651" s="9"/>
-      <c r="I651" s="9"/>
-      <c r="J651" s="7" t="s">
-        <v>558</v>
-      </c>
-      <c r="K651" s="7" t="s">
+      <c r="H651" s="2"/>
+      <c r="I651" s="2"/>
+      <c r="J651" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="K651" s="1"/>
+      <c r="L651" s="1"/>
+      <c r="M651" s="1"/>
+      <c r="N651" s="1"/>
+      <c r="O651" s="1"/>
+    </row>
+    <row r="652" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A652" s="1"/>
+      <c r="B652" s="1"/>
+      <c r="C652" s="1"/>
+      <c r="D652" s="1"/>
+      <c r="E652" s="2"/>
+      <c r="F652" s="2"/>
+      <c r="G652" s="2"/>
+      <c r="H652" s="2"/>
+      <c r="I652" s="2"/>
+      <c r="J652" s="1"/>
+      <c r="K652" s="1"/>
+      <c r="L652" s="1"/>
+      <c r="M652" s="1"/>
+      <c r="N652" s="1"/>
+      <c r="O652" s="1"/>
+    </row>
+    <row r="653" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A653" s="1"/>
+      <c r="B653" s="1"/>
+      <c r="C653" s="1"/>
+      <c r="D653" s="1"/>
+      <c r="E653" s="2"/>
+      <c r="F653" s="2"/>
+      <c r="G653" s="2"/>
+      <c r="H653" s="2"/>
+      <c r="I653" s="2"/>
+      <c r="J653" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="K653" s="1"/>
+      <c r="L653" s="1"/>
+      <c r="M653" s="1"/>
+      <c r="N653" s="1"/>
+      <c r="O653" s="1"/>
+    </row>
+    <row r="654" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B654" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C654" s="13" t="s">
+        <v>561</v>
+      </c>
+      <c r="D654" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="E654" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="F654" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G654" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H654" s="14"/>
+      <c r="I654" s="14"/>
+      <c r="J654" s="13" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="655" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A655" s="1"/>
+      <c r="B655" s="1"/>
+      <c r="C655" s="1"/>
+      <c r="D655" s="1"/>
+      <c r="E655" s="2"/>
+      <c r="F655" s="2"/>
+      <c r="G655" s="2"/>
+      <c r="H655" s="2"/>
+      <c r="I655" s="2"/>
+      <c r="J655" s="1"/>
+      <c r="K655" s="1"/>
+      <c r="L655" s="1"/>
+      <c r="M655" s="1"/>
+      <c r="N655" s="1"/>
+      <c r="O655" s="1"/>
+    </row>
+    <row r="656" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A656" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B656" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C656" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="D656" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="E656" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F656" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G656" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H656" s="14"/>
+      <c r="I656" s="14"/>
+      <c r="J656" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="K656" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="652" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B652" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="C652" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="D652" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="E652" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="F652" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G652" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H652" s="9"/>
-      <c r="I652" s="9"/>
-      <c r="J652" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="K652" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="653" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B653" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C653" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D653" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E653" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="F653" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G653" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H653" s="9"/>
-      <c r="I653" s="9"/>
-      <c r="J653" s="7" t="s">
-        <v>554</v>
-      </c>
-      <c r="K653" s="7" t="s">
+    <row r="657" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A657" s="10"/>
+      <c r="B657" s="10"/>
+      <c r="C657" s="10"/>
+      <c r="D657" s="10"/>
+      <c r="E657" s="11"/>
+      <c r="F657" s="11"/>
+      <c r="G657" s="11"/>
+      <c r="H657" s="11"/>
+      <c r="I657" s="11"/>
+      <c r="J657" s="10"/>
+      <c r="K657" s="10"/>
+      <c r="L657" s="10"/>
+      <c r="M657" s="10"/>
+      <c r="N657" s="10"/>
+      <c r="O657" s="10"/>
+    </row>
+    <row r="658" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A658" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B658" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C658" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="D658" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="E658" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F658" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G658" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H658" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I658" s="14"/>
+      <c r="J658" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="K658" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="654" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A654" s="1"/>
-      <c r="B654" s="1"/>
-      <c r="C654" s="1"/>
-      <c r="D654" s="1"/>
-      <c r="E654" s="2"/>
-      <c r="F654" s="2"/>
-      <c r="G654" s="2"/>
-      <c r="H654" s="2"/>
-      <c r="I654" s="2"/>
-      <c r="J654" s="1"/>
-      <c r="K654" s="1"/>
-      <c r="L654" s="1"/>
-      <c r="M654" s="1"/>
-      <c r="N654" s="1"/>
-      <c r="O654" s="1"/>
-    </row>
-    <row r="655" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A655" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B655" s="13" t="s">
-        <v>559</v>
-      </c>
-      <c r="C655" s="13" t="s">
-        <v>560</v>
-      </c>
-      <c r="D655" s="13" t="s">
-        <v>561</v>
-      </c>
-      <c r="E655" s="14" t="s">
-        <v>562</v>
-      </c>
-      <c r="F655" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G655" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H655" s="14"/>
-      <c r="I655" s="14"/>
-      <c r="J655" s="13" t="s">
-        <v>563</v>
-      </c>
-      <c r="K655" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="656" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A656" s="10"/>
-      <c r="B656" s="10"/>
-      <c r="C656" s="10"/>
-      <c r="D656" s="10"/>
-      <c r="E656" s="11"/>
-      <c r="F656" s="11"/>
-      <c r="G656" s="11"/>
-      <c r="H656" s="11"/>
-      <c r="I656" s="11"/>
-      <c r="J656" s="10"/>
-      <c r="K656" s="10"/>
-      <c r="L656" s="10"/>
-      <c r="M656" s="10"/>
-      <c r="N656" s="10"/>
-      <c r="O656" s="10"/>
-    </row>
-    <row r="657" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A657" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B657" s="13" t="s">
-        <v>389</v>
-      </c>
-      <c r="C657" s="13" t="s">
-        <v>390</v>
-      </c>
-      <c r="D657" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="E657" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F657" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G657" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H657" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="I657" s="14"/>
-      <c r="J657" s="13" t="s">
-        <v>392</v>
-      </c>
-      <c r="K657" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="658" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A658" s="1"/>
-      <c r="B658" s="1"/>
-      <c r="C658" s="1"/>
-      <c r="D658" s="1"/>
-      <c r="E658" s="2"/>
-      <c r="F658" s="2"/>
-      <c r="G658" s="2"/>
-      <c r="H658" s="2"/>
-      <c r="I658" s="2"/>
-      <c r="J658" s="1"/>
-      <c r="K658" s="1"/>
-      <c r="L658" s="1"/>
-      <c r="M658" s="1"/>
-      <c r="N658" s="1"/>
-      <c r="O658" s="1"/>
-    </row>
     <row r="659" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A659" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A659" s="1"/>
       <c r="B659" s="1"/>
       <c r="C659" s="1"/>
       <c r="D659" s="1"/>
@@ -15113,7 +15093,9 @@
       <c r="O659" s="1"/>
     </row>
     <row r="660" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A660" s="1"/>
+      <c r="A660" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B660" s="1"/>
       <c r="C660" s="1"/>
       <c r="D660" s="1"/>
@@ -15122,9 +15104,7 @@
       <c r="G660" s="2"/>
       <c r="H660" s="2"/>
       <c r="I660" s="2"/>
-      <c r="J660" s="1" t="s">
-        <v>504</v>
-      </c>
+      <c r="J660" s="1"/>
       <c r="K660" s="1"/>
       <c r="L660" s="1"/>
       <c r="M660" s="1"/>
@@ -15142,7 +15122,7 @@
       <c r="H661" s="2"/>
       <c r="I661" s="2"/>
       <c r="J661" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K661" s="1"/>
       <c r="L661" s="1"/>
@@ -15161,7 +15141,7 @@
       <c r="H662" s="2"/>
       <c r="I662" s="2"/>
       <c r="J662" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K662" s="1"/>
       <c r="L662" s="1"/>
@@ -15179,7 +15159,9 @@
       <c r="G663" s="2"/>
       <c r="H663" s="2"/>
       <c r="I663" s="2"/>
-      <c r="J663" s="1"/>
+      <c r="J663" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="K663" s="1"/>
       <c r="L663" s="1"/>
       <c r="M663" s="1"/>
@@ -15188,83 +15170,86 @@
     </row>
     <row r="664" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="1"/>
-      <c r="B664" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="C664" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="D664" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="E664" s="9" t="n">
-        <v>45692</v>
-      </c>
-      <c r="F664" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G664" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="B664" s="1"/>
+      <c r="C664" s="1"/>
+      <c r="D664" s="1"/>
+      <c r="E664" s="2"/>
+      <c r="F664" s="2"/>
+      <c r="G664" s="2"/>
       <c r="H664" s="2"/>
       <c r="I664" s="2"/>
-      <c r="J664" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="K664" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="J664" s="1"/>
+      <c r="K664" s="1"/>
       <c r="L664" s="1"/>
       <c r="M664" s="1"/>
       <c r="N664" s="1"/>
       <c r="O664" s="1"/>
     </row>
-    <row r="665" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A665" s="1"/>
-      <c r="B665" s="1"/>
-      <c r="C665" s="1"/>
-      <c r="D665" s="1"/>
-      <c r="E665" s="2"/>
-      <c r="F665" s="2"/>
-      <c r="G665" s="2"/>
-      <c r="H665" s="2"/>
-      <c r="I665" s="2"/>
-      <c r="J665" s="1"/>
-      <c r="K665" s="1"/>
-      <c r="L665" s="1"/>
-      <c r="M665" s="1"/>
-      <c r="N665" s="1"/>
-      <c r="O665" s="1"/>
-    </row>
-    <row r="666" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A666" s="1"/>
-      <c r="B666" s="1"/>
-      <c r="C666" s="1"/>
-      <c r="D666" s="1"/>
-      <c r="E666" s="2"/>
-      <c r="F666" s="2"/>
-      <c r="G666" s="2"/>
-      <c r="H666" s="2"/>
-      <c r="I666" s="2"/>
-      <c r="J666" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="K666" s="1"/>
-      <c r="L666" s="1"/>
-      <c r="M666" s="1"/>
-      <c r="N666" s="1"/>
-      <c r="O666" s="1"/>
-    </row>
-    <row r="667" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A667" s="1"/>
+    <row r="665" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B665" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="C665" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="D665" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="E665" s="9" t="n">
+        <v>45692</v>
+      </c>
+      <c r="F665" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G665" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H665" s="9"/>
+      <c r="I665" s="9"/>
+      <c r="J665" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="K665" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="666" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B666" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C666" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D666" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="E666" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="F666" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="G666" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H666" s="9"/>
+      <c r="I666" s="9"/>
+      <c r="J666" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="K666" s="7" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="667" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B667" s="7" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
       <c r="C667" s="7" t="s">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="D667" s="7" t="s">
-        <v>116</v>
+        <v>166</v>
       </c>
       <c r="E667" s="9" t="s">
         <v>97</v>
@@ -15275,27 +15260,24 @@
       <c r="G667" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H667" s="2"/>
-      <c r="I667" s="2"/>
-      <c r="J667" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="K667" s="1"/>
-      <c r="L667" s="1"/>
-      <c r="M667" s="1"/>
-      <c r="N667" s="1"/>
-      <c r="O667" s="1"/>
-    </row>
-    <row r="668" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A668" s="1"/>
+      <c r="H667" s="9"/>
+      <c r="I667" s="9"/>
+      <c r="J667" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="K667" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="668" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B668" s="13" t="s">
-        <v>283</v>
+        <v>529</v>
       </c>
       <c r="C668" s="13" t="s">
-        <v>284</v>
+        <v>530</v>
       </c>
       <c r="D668" s="13" t="s">
-        <v>285</v>
+        <v>531</v>
       </c>
       <c r="E668" s="14" t="s">
         <v>97</v>
@@ -15306,27 +15288,24 @@
       <c r="G668" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H668" s="2"/>
-      <c r="I668" s="2"/>
-      <c r="J668" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="K668" s="1"/>
-      <c r="L668" s="1"/>
-      <c r="M668" s="1"/>
-      <c r="N668" s="1"/>
-      <c r="O668" s="1"/>
-    </row>
-    <row r="669" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A669" s="1"/>
+      <c r="H668" s="14"/>
+      <c r="I668" s="14"/>
+      <c r="J668" s="13" t="s">
+        <v>564</v>
+      </c>
+      <c r="K668" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="669" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B669" s="7" t="s">
-        <v>164</v>
+        <v>482</v>
       </c>
       <c r="C669" s="7" t="s">
-        <v>165</v>
+        <v>483</v>
       </c>
       <c r="D669" s="7" t="s">
-        <v>166</v>
+        <v>484</v>
       </c>
       <c r="E669" s="9" t="s">
         <v>97</v>
@@ -15337,65 +15316,83 @@
       <c r="G669" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H669" s="2"/>
-      <c r="I669" s="2"/>
-      <c r="J669" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="K669" s="1"/>
-      <c r="L669" s="1"/>
-      <c r="M669" s="1"/>
-      <c r="N669" s="1"/>
-      <c r="O669" s="1"/>
-    </row>
-    <row r="670" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A670" s="1"/>
-      <c r="B670" s="1"/>
-      <c r="C670" s="1"/>
-      <c r="D670" s="1"/>
-      <c r="E670" s="2"/>
-      <c r="F670" s="2"/>
-      <c r="G670" s="2"/>
-      <c r="H670" s="2"/>
-      <c r="I670" s="2"/>
-      <c r="J670" s="1"/>
-      <c r="K670" s="1"/>
-      <c r="L670" s="1"/>
-      <c r="M670" s="1"/>
-      <c r="N670" s="1"/>
-      <c r="O670" s="1"/>
-    </row>
-    <row r="671" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A671" s="1"/>
-      <c r="B671" s="1"/>
-      <c r="C671" s="1"/>
-      <c r="D671" s="1"/>
-      <c r="E671" s="2"/>
-      <c r="F671" s="2"/>
-      <c r="G671" s="2"/>
-      <c r="H671" s="2"/>
-      <c r="I671" s="2"/>
-      <c r="J671" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="K671" s="1"/>
-      <c r="L671" s="1"/>
-      <c r="M671" s="1"/>
-      <c r="N671" s="1"/>
-      <c r="O671" s="1"/>
+      <c r="H669" s="9"/>
+      <c r="I669" s="9"/>
+      <c r="J669" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="K669" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="670" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B670" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C670" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D670" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E670" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F670" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G670" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H670" s="9"/>
+      <c r="I670" s="9"/>
+      <c r="J670" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K670" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="671" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B671" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C671" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="D671" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="E671" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="F671" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G671" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H671" s="9"/>
+      <c r="I671" s="9"/>
+      <c r="J671" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="K671" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="672" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B672" s="13" t="s">
-        <v>384</v>
+        <v>192</v>
       </c>
       <c r="C672" s="13" t="s">
-        <v>569</v>
+        <v>193</v>
       </c>
       <c r="D672" s="13" t="s">
-        <v>386</v>
+        <v>194</v>
       </c>
       <c r="E672" s="14" t="s">
-        <v>387</v>
+        <v>195</v>
       </c>
       <c r="F672" s="14" t="s">
         <v>9</v>
@@ -15406,44 +15403,55 @@
       <c r="H672" s="14"/>
       <c r="I672" s="14"/>
       <c r="J672" s="13" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="673" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A673" s="1"/>
-      <c r="B673" s="1"/>
-      <c r="C673" s="1"/>
-      <c r="D673" s="1"/>
-      <c r="E673" s="2"/>
-      <c r="F673" s="2"/>
-      <c r="G673" s="2"/>
-      <c r="H673" s="2"/>
-      <c r="I673" s="2"/>
-      <c r="J673" s="1"/>
-      <c r="K673" s="1"/>
-      <c r="L673" s="1"/>
-      <c r="M673" s="1"/>
-      <c r="N673" s="1"/>
-      <c r="O673" s="1"/>
-    </row>
-    <row r="674" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A674" s="13" t="s">
-        <v>13</v>
-      </c>
+        <v>565</v>
+      </c>
+      <c r="K672" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="673" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B673" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C673" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D673" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E673" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F673" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G673" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H673" s="9"/>
+      <c r="I673" s="9"/>
+      <c r="J673" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K673" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="674" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B674" s="13" t="s">
-        <v>354</v>
+        <v>376</v>
       </c>
       <c r="C674" s="13" t="s">
-        <v>355</v>
+        <v>377</v>
       </c>
       <c r="D674" s="13" t="s">
-        <v>356</v>
+        <v>295</v>
       </c>
       <c r="E674" s="14" t="s">
-        <v>97</v>
+        <v>378</v>
       </c>
       <c r="F674" s="14" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="G674" s="14" t="s">
         <v>10</v>
@@ -15451,64 +15459,61 @@
       <c r="H674" s="14"/>
       <c r="I674" s="14"/>
       <c r="J674" s="13" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
       <c r="K674" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="675" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B675" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="C675" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="D675" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="E675" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="F675" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G675" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H675" s="14"/>
+      <c r="I675" s="14"/>
+      <c r="J675" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="K675" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="675" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A675" s="10"/>
-      <c r="B675" s="10"/>
-      <c r="C675" s="10"/>
-      <c r="D675" s="10"/>
-      <c r="E675" s="11"/>
-      <c r="F675" s="11"/>
-      <c r="G675" s="11"/>
-      <c r="H675" s="11"/>
-      <c r="I675" s="11"/>
-      <c r="J675" s="10"/>
-      <c r="K675" s="10"/>
-      <c r="L675" s="10"/>
-      <c r="M675" s="10"/>
-      <c r="N675" s="10"/>
-      <c r="O675" s="10"/>
-    </row>
-    <row r="676" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A676" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B676" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="C676" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="D676" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="E676" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F676" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G676" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H676" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="I676" s="14"/>
-      <c r="J676" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="K676" s="13" t="s">
-        <v>43</v>
-      </c>
+    <row r="676" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A676" s="1"/>
+      <c r="B676" s="1"/>
+      <c r="C676" s="1"/>
+      <c r="D676" s="1"/>
+      <c r="E676" s="2"/>
+      <c r="F676" s="2"/>
+      <c r="G676" s="2"/>
+      <c r="H676" s="2"/>
+      <c r="I676" s="2"/>
+      <c r="J676" s="1"/>
+      <c r="K676" s="1"/>
+      <c r="L676" s="1"/>
+      <c r="M676" s="1"/>
+      <c r="N676" s="1"/>
+      <c r="O676" s="1"/>
     </row>
     <row r="677" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A677" s="1"/>
+      <c r="A677" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B677" s="1"/>
       <c r="C677" s="1"/>
       <c r="D677" s="1"/>
@@ -15524,24 +15529,33 @@
       <c r="N677" s="1"/>
       <c r="O677" s="1"/>
     </row>
-    <row r="678" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A678" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B678" s="1"/>
-      <c r="C678" s="1"/>
-      <c r="D678" s="1"/>
-      <c r="E678" s="2"/>
-      <c r="F678" s="2"/>
-      <c r="G678" s="2"/>
-      <c r="H678" s="2"/>
-      <c r="I678" s="2"/>
-      <c r="J678" s="1"/>
-      <c r="K678" s="1"/>
-      <c r="L678" s="1"/>
-      <c r="M678" s="1"/>
-      <c r="N678" s="1"/>
-      <c r="O678" s="1"/>
+    <row r="678" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B678" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C678" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="D678" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="E678" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F678" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G678" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H678" s="14"/>
+      <c r="I678" s="14"/>
+      <c r="J678" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="K678" s="13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="679" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="1"/>
@@ -15553,52 +15567,62 @@
       <c r="G679" s="2"/>
       <c r="H679" s="2"/>
       <c r="I679" s="2"/>
-      <c r="J679" s="1" t="s">
-        <v>504</v>
-      </c>
+      <c r="J679" s="1"/>
       <c r="K679" s="1"/>
       <c r="L679" s="1"/>
       <c r="M679" s="1"/>
       <c r="N679" s="1"/>
       <c r="O679" s="1"/>
     </row>
-    <row r="680" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A680" s="1"/>
-      <c r="B680" s="1"/>
-      <c r="C680" s="1"/>
-      <c r="D680" s="1"/>
-      <c r="E680" s="2"/>
-      <c r="F680" s="2"/>
-      <c r="G680" s="2"/>
-      <c r="H680" s="2"/>
-      <c r="I680" s="2"/>
-      <c r="J680" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="K680" s="1"/>
-      <c r="L680" s="1"/>
-      <c r="M680" s="1"/>
-      <c r="N680" s="1"/>
-      <c r="O680" s="1"/>
-    </row>
-    <row r="681" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A681" s="1"/>
-      <c r="B681" s="1"/>
-      <c r="C681" s="1"/>
-      <c r="D681" s="1"/>
-      <c r="E681" s="2"/>
-      <c r="F681" s="2"/>
-      <c r="G681" s="2"/>
-      <c r="H681" s="2"/>
-      <c r="I681" s="2"/>
-      <c r="J681" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="K681" s="1"/>
-      <c r="L681" s="1"/>
-      <c r="M681" s="1"/>
-      <c r="N681" s="1"/>
-      <c r="O681" s="1"/>
+    <row r="680" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A680" s="10"/>
+      <c r="B680" s="10"/>
+      <c r="C680" s="10"/>
+      <c r="D680" s="10"/>
+      <c r="E680" s="11"/>
+      <c r="F680" s="11"/>
+      <c r="G680" s="11"/>
+      <c r="H680" s="11"/>
+      <c r="I680" s="11"/>
+      <c r="J680" s="10"/>
+      <c r="K680" s="10"/>
+      <c r="L680" s="10"/>
+      <c r="M680" s="10"/>
+      <c r="N680" s="10"/>
+      <c r="O680" s="10"/>
+    </row>
+    <row r="681" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A681" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B681" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C681" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D681" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E681" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F681" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G681" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H681" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I681" s="9"/>
+      <c r="J681" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="K681" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="682" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="1"/>
@@ -15617,394 +15641,323 @@
       <c r="N682" s="1"/>
       <c r="O682" s="1"/>
     </row>
-    <row r="683" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B683" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="C683" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="D683" s="7" t="s">
-        <v>464</v>
-      </c>
-      <c r="E683" s="9" t="n">
-        <v>45692</v>
-      </c>
-      <c r="F683" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G683" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H683" s="9"/>
-      <c r="I683" s="9"/>
-      <c r="J683" s="7" t="s">
-        <v>520</v>
-      </c>
-      <c r="K683" s="7" t="s">
+    <row r="683" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A683" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B683" s="1"/>
+      <c r="C683" s="1"/>
+      <c r="D683" s="1"/>
+      <c r="E683" s="2"/>
+      <c r="F683" s="2"/>
+      <c r="G683" s="2"/>
+      <c r="H683" s="2"/>
+      <c r="I683" s="2"/>
+      <c r="J683" s="1"/>
+      <c r="K683" s="1"/>
+      <c r="L683" s="1"/>
+      <c r="M683" s="1"/>
+      <c r="N683" s="1"/>
+      <c r="O683" s="1"/>
+    </row>
+    <row r="684" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A684" s="1"/>
+      <c r="B684" s="1"/>
+      <c r="C684" s="1"/>
+      <c r="D684" s="1"/>
+      <c r="E684" s="2"/>
+      <c r="F684" s="2"/>
+      <c r="G684" s="2"/>
+      <c r="H684" s="2"/>
+      <c r="I684" s="2"/>
+      <c r="J684" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="K684" s="1"/>
+      <c r="L684" s="1"/>
+      <c r="M684" s="1"/>
+      <c r="N684" s="1"/>
+      <c r="O684" s="1"/>
+    </row>
+    <row r="685" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A685" s="1"/>
+      <c r="B685" s="1"/>
+      <c r="C685" s="1"/>
+      <c r="D685" s="1"/>
+      <c r="E685" s="2"/>
+      <c r="F685" s="2"/>
+      <c r="G685" s="2"/>
+      <c r="H685" s="2"/>
+      <c r="I685" s="2"/>
+      <c r="J685" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="K685" s="1"/>
+      <c r="L685" s="1"/>
+      <c r="M685" s="1"/>
+      <c r="N685" s="1"/>
+      <c r="O685" s="1"/>
+    </row>
+    <row r="686" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A686" s="1"/>
+      <c r="B686" s="1"/>
+      <c r="C686" s="1"/>
+      <c r="D686" s="1"/>
+      <c r="E686" s="2"/>
+      <c r="F686" s="2"/>
+      <c r="G686" s="2"/>
+      <c r="H686" s="2"/>
+      <c r="I686" s="2"/>
+      <c r="J686" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="K686" s="1"/>
+      <c r="L686" s="1"/>
+      <c r="M686" s="1"/>
+      <c r="N686" s="1"/>
+      <c r="O686" s="1"/>
+    </row>
+    <row r="687" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A687" s="1"/>
+      <c r="B687" s="1"/>
+      <c r="C687" s="1"/>
+      <c r="D687" s="1"/>
+      <c r="E687" s="2"/>
+      <c r="F687" s="2"/>
+      <c r="G687" s="2"/>
+      <c r="H687" s="2"/>
+      <c r="I687" s="2"/>
+      <c r="J687" s="1"/>
+      <c r="K687" s="1"/>
+      <c r="L687" s="1"/>
+      <c r="M687" s="1"/>
+      <c r="N687" s="1"/>
+      <c r="O687" s="1"/>
+    </row>
+    <row r="688" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A688" s="1"/>
+      <c r="B688" s="1"/>
+      <c r="C688" s="1"/>
+      <c r="D688" s="1"/>
+      <c r="E688" s="2"/>
+      <c r="F688" s="2"/>
+      <c r="G688" s="2"/>
+      <c r="H688" s="2"/>
+      <c r="I688" s="2"/>
+      <c r="J688" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="K688" s="1"/>
+      <c r="L688" s="1"/>
+      <c r="M688" s="1"/>
+      <c r="N688" s="1"/>
+      <c r="O688" s="1"/>
+    </row>
+    <row r="689" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A689" s="1"/>
+      <c r="B689" s="1"/>
+      <c r="C689" s="1"/>
+      <c r="D689" s="1"/>
+      <c r="E689" s="2"/>
+      <c r="F689" s="2"/>
+      <c r="G689" s="2"/>
+      <c r="H689" s="2"/>
+      <c r="I689" s="2"/>
+      <c r="J689" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="K689" s="1"/>
+      <c r="L689" s="1"/>
+      <c r="M689" s="1"/>
+      <c r="N689" s="1"/>
+      <c r="O689" s="1"/>
+    </row>
+    <row r="690" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A690" s="1"/>
+      <c r="B690" s="1"/>
+      <c r="C690" s="1"/>
+      <c r="D690" s="1"/>
+      <c r="E690" s="2"/>
+      <c r="F690" s="2"/>
+      <c r="G690" s="2"/>
+      <c r="H690" s="2"/>
+      <c r="I690" s="2"/>
+      <c r="J690" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K690" s="1"/>
+      <c r="L690" s="1"/>
+      <c r="M690" s="1"/>
+      <c r="N690" s="1"/>
+      <c r="O690" s="1"/>
+    </row>
+    <row r="691" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A691" s="1"/>
+      <c r="B691" s="1"/>
+      <c r="C691" s="1"/>
+      <c r="D691" s="1"/>
+      <c r="E691" s="2"/>
+      <c r="F691" s="2"/>
+      <c r="G691" s="2"/>
+      <c r="H691" s="2"/>
+      <c r="I691" s="2"/>
+      <c r="J691" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="K691" s="1"/>
+      <c r="L691" s="1"/>
+      <c r="M691" s="1"/>
+      <c r="N691" s="1"/>
+      <c r="O691" s="1"/>
+    </row>
+    <row r="692" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A692" s="1"/>
+      <c r="B692" s="1"/>
+      <c r="C692" s="1"/>
+      <c r="D692" s="1"/>
+      <c r="E692" s="2"/>
+      <c r="F692" s="2"/>
+      <c r="G692" s="2"/>
+      <c r="H692" s="2"/>
+      <c r="I692" s="2"/>
+      <c r="J692" s="1"/>
+      <c r="K692" s="1"/>
+      <c r="L692" s="1"/>
+      <c r="M692" s="1"/>
+      <c r="N692" s="1"/>
+      <c r="O692" s="1"/>
+    </row>
+    <row r="693" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B693" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="C693" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="D693" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="E693" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="F693" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="G693" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H693" s="9"/>
+      <c r="I693" s="9"/>
+      <c r="J693" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="K693" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="684" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B684" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C684" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="D684" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="E684" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="F684" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="G684" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H684" s="9"/>
-      <c r="I684" s="9"/>
-      <c r="J684" s="7" t="s">
-        <v>570</v>
-      </c>
-      <c r="K684" s="7" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="685" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B685" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C685" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D685" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E685" s="9" t="s">
+    <row r="694" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B694" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C694" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D694" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E694" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F685" s="9" t="s">
+      <c r="F694" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G685" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H685" s="9"/>
-      <c r="I685" s="9"/>
-      <c r="J685" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="K685" s="7" t="s">
+      <c r="G694" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H694" s="9"/>
+      <c r="I694" s="9"/>
+      <c r="J694" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K694" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="686" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B686" s="13" t="s">
-        <v>529</v>
-      </c>
-      <c r="C686" s="13" t="s">
-        <v>530</v>
-      </c>
-      <c r="D686" s="13" t="s">
-        <v>531</v>
-      </c>
-      <c r="E686" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F686" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G686" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H686" s="14"/>
-      <c r="I686" s="14"/>
-      <c r="J686" s="13" t="s">
-        <v>572</v>
-      </c>
-      <c r="K686" s="13" t="s">
+    <row r="695" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B695" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C695" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D695" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="E695" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="F695" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G695" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H695" s="9"/>
+      <c r="I695" s="9"/>
+      <c r="J695" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="K695" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="696" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A696" s="1"/>
+      <c r="B696" s="1"/>
+      <c r="C696" s="1"/>
+      <c r="D696" s="1"/>
+      <c r="E696" s="2"/>
+      <c r="F696" s="2"/>
+      <c r="G696" s="2"/>
+      <c r="H696" s="2"/>
+      <c r="I696" s="2"/>
+      <c r="J696" s="1"/>
+      <c r="K696" s="1"/>
+      <c r="L696" s="1"/>
+      <c r="M696" s="1"/>
+      <c r="N696" s="1"/>
+      <c r="O696" s="1"/>
+    </row>
+    <row r="697" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A697" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B697" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="C697" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="D697" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="E697" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F697" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G697" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H697" s="9"/>
+      <c r="I697" s="9"/>
+      <c r="J697" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="K697" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="687" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B687" s="7" t="s">
-        <v>482</v>
-      </c>
-      <c r="C687" s="7" t="s">
-        <v>483</v>
-      </c>
-      <c r="D687" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="E687" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F687" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G687" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H687" s="9"/>
-      <c r="I687" s="9"/>
-      <c r="J687" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="K687" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="688" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B688" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C688" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D688" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E688" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F688" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G688" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H688" s="9"/>
-      <c r="I688" s="9"/>
-      <c r="J688" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="K688" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="689" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B689" s="7" t="s">
-        <v>466</v>
-      </c>
-      <c r="C689" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="D689" s="7" t="s">
-        <v>468</v>
-      </c>
-      <c r="E689" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="F689" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G689" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H689" s="9"/>
-      <c r="I689" s="9"/>
-      <c r="J689" s="7" t="s">
-        <v>523</v>
-      </c>
-      <c r="K689" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="690" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B690" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C690" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="D690" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="E690" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="F690" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G690" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H690" s="14"/>
-      <c r="I690" s="14"/>
-      <c r="J690" s="13" t="s">
-        <v>573</v>
-      </c>
-      <c r="K690" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="691" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B691" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C691" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D691" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E691" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="F691" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G691" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H691" s="9"/>
-      <c r="I691" s="9"/>
-      <c r="J691" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="K691" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="692" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B692" s="13" t="s">
-        <v>376</v>
-      </c>
-      <c r="C692" s="13" t="s">
-        <v>377</v>
-      </c>
-      <c r="D692" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="E692" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="F692" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G692" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H692" s="14"/>
-      <c r="I692" s="14"/>
-      <c r="J692" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="K692" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="693" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B693" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="C693" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="D693" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="E693" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="F693" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G693" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H693" s="14"/>
-      <c r="I693" s="14"/>
-      <c r="J693" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="K693" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="694" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A694" s="1"/>
-      <c r="B694" s="1"/>
-      <c r="C694" s="1"/>
-      <c r="D694" s="1"/>
-      <c r="E694" s="2"/>
-      <c r="F694" s="2"/>
-      <c r="G694" s="2"/>
-      <c r="H694" s="2"/>
-      <c r="I694" s="2"/>
-      <c r="J694" s="1"/>
-      <c r="K694" s="1"/>
-      <c r="L694" s="1"/>
-      <c r="M694" s="1"/>
-      <c r="N694" s="1"/>
-      <c r="O694" s="1"/>
-    </row>
-    <row r="695" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A695" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B695" s="1"/>
-      <c r="C695" s="1"/>
-      <c r="D695" s="1"/>
-      <c r="E695" s="2"/>
-      <c r="F695" s="2"/>
-      <c r="G695" s="2"/>
-      <c r="H695" s="2"/>
-      <c r="I695" s="2"/>
-      <c r="J695" s="1"/>
-      <c r="K695" s="1"/>
-      <c r="L695" s="1"/>
-      <c r="M695" s="1"/>
-      <c r="N695" s="1"/>
-      <c r="O695" s="1"/>
-    </row>
-    <row r="696" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B696" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="C696" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="D696" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="E696" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F696" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G696" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H696" s="14"/>
-      <c r="I696" s="14"/>
-      <c r="J696" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="K696" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="697" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A697" s="1"/>
-      <c r="B697" s="1"/>
-      <c r="C697" s="1"/>
-      <c r="D697" s="1"/>
-      <c r="E697" s="2"/>
-      <c r="F697" s="2"/>
-      <c r="G697" s="2"/>
-      <c r="H697" s="2"/>
-      <c r="I697" s="2"/>
-      <c r="J697" s="1"/>
-      <c r="K697" s="1"/>
-      <c r="L697" s="1"/>
-      <c r="M697" s="1"/>
-      <c r="N697" s="1"/>
-      <c r="O697" s="1"/>
     </row>
     <row r="698" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A698" s="10"/>
@@ -16023,36 +15976,36 @@
       <c r="N698" s="10"/>
       <c r="O698" s="10"/>
     </row>
-    <row r="699" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A699" s="7" t="s">
+    <row r="699" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A699" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B699" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C699" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D699" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="E699" s="9" t="s">
+      <c r="B699" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C699" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="D699" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="E699" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F699" s="9" t="s">
+      <c r="F699" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G699" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H699" s="9" t="s">
+      <c r="G699" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H699" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="I699" s="9"/>
-      <c r="J699" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="K699" s="7" t="s">
+      <c r="I699" s="14"/>
+      <c r="J699" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="K699" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -16166,114 +16119,161 @@
       <c r="N705" s="1"/>
       <c r="O705" s="1"/>
     </row>
-    <row r="706" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A706" s="1"/>
-      <c r="B706" s="1"/>
-      <c r="C706" s="1"/>
-      <c r="D706" s="1"/>
-      <c r="E706" s="2"/>
-      <c r="F706" s="2"/>
-      <c r="G706" s="2"/>
-      <c r="H706" s="2"/>
-      <c r="I706" s="2"/>
-      <c r="J706" s="1" t="s">
+    <row r="706" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B706" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="C706" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="D706" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="E706" s="9" t="n">
+        <v>45692</v>
+      </c>
+      <c r="F706" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G706" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H706" s="9"/>
+      <c r="I706" s="9"/>
+      <c r="J706" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="K706" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="707" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B707" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C707" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D707" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E707" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F707" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G707" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H707" s="9"/>
+      <c r="I707" s="9"/>
+      <c r="J707" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="K707" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="708" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B708" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="C708" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="D708" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="E708" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F708" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G708" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H708" s="9"/>
+      <c r="I708" s="9"/>
+      <c r="J708" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="K708" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="709" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B709" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="C709" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="D709" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="E709" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F709" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G709" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H709" s="9"/>
+      <c r="I709" s="9"/>
+      <c r="J709" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="K709" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="710" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B710" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C710" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D710" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E710" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F710" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G710" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H710" s="9"/>
+      <c r="I710" s="9"/>
+      <c r="J710" s="7" t="s">
         <v>574</v>
       </c>
-      <c r="K706" s="1"/>
-      <c r="L706" s="1"/>
-      <c r="M706" s="1"/>
-      <c r="N706" s="1"/>
-      <c r="O706" s="1"/>
-    </row>
-    <row r="707" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A707" s="1"/>
-      <c r="B707" s="1"/>
-      <c r="C707" s="1"/>
-      <c r="D707" s="1"/>
-      <c r="E707" s="2"/>
-      <c r="F707" s="2"/>
-      <c r="G707" s="2"/>
-      <c r="H707" s="2"/>
-      <c r="I707" s="2"/>
-      <c r="J707" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="K707" s="1"/>
-      <c r="L707" s="1"/>
-      <c r="M707" s="1"/>
-      <c r="N707" s="1"/>
-      <c r="O707" s="1"/>
-    </row>
-    <row r="708" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A708" s="1"/>
-      <c r="B708" s="1"/>
-      <c r="C708" s="1"/>
-      <c r="D708" s="1"/>
-      <c r="E708" s="2"/>
-      <c r="F708" s="2"/>
-      <c r="G708" s="2"/>
-      <c r="H708" s="2"/>
-      <c r="I708" s="2"/>
-      <c r="J708" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="K708" s="1"/>
-      <c r="L708" s="1"/>
-      <c r="M708" s="1"/>
-      <c r="N708" s="1"/>
-      <c r="O708" s="1"/>
-    </row>
-    <row r="709" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A709" s="1"/>
-      <c r="B709" s="1"/>
-      <c r="C709" s="1"/>
-      <c r="D709" s="1"/>
-      <c r="E709" s="2"/>
-      <c r="F709" s="2"/>
-      <c r="G709" s="2"/>
-      <c r="H709" s="2"/>
-      <c r="I709" s="2"/>
-      <c r="J709" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="K709" s="1"/>
-      <c r="L709" s="1"/>
-      <c r="M709" s="1"/>
-      <c r="N709" s="1"/>
-      <c r="O709" s="1"/>
-    </row>
-    <row r="710" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A710" s="1"/>
-      <c r="B710" s="1"/>
-      <c r="C710" s="1"/>
-      <c r="D710" s="1"/>
-      <c r="E710" s="2"/>
-      <c r="F710" s="2"/>
-      <c r="G710" s="2"/>
-      <c r="H710" s="2"/>
-      <c r="I710" s="2"/>
-      <c r="J710" s="1"/>
-      <c r="K710" s="1"/>
-      <c r="L710" s="1"/>
-      <c r="M710" s="1"/>
-      <c r="N710" s="1"/>
-      <c r="O710" s="1"/>
+      <c r="K710" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="711" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B711" s="7" t="s">
-        <v>576</v>
+        <v>183</v>
       </c>
       <c r="C711" s="7" t="s">
-        <v>577</v>
+        <v>184</v>
       </c>
       <c r="D711" s="7" t="s">
-        <v>578</v>
+        <v>185</v>
       </c>
       <c r="E711" s="9" t="s">
-        <v>579</v>
+        <v>97</v>
       </c>
       <c r="F711" s="9" t="s">
-        <v>256</v>
+        <v>41</v>
       </c>
       <c r="G711" s="9" t="s">
         <v>10</v>
@@ -16281,7 +16281,7 @@
       <c r="H711" s="9"/>
       <c r="I711" s="9"/>
       <c r="J711" s="7" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K711" s="7" t="s">
         <v>43</v>
@@ -16289,19 +16289,19 @@
     </row>
     <row r="712" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B712" s="7" t="s">
-        <v>114</v>
+        <v>277</v>
       </c>
       <c r="C712" s="7" t="s">
-        <v>115</v>
+        <v>278</v>
       </c>
       <c r="D712" s="7" t="s">
-        <v>116</v>
+        <v>279</v>
       </c>
       <c r="E712" s="9" t="s">
-        <v>97</v>
+        <v>280</v>
       </c>
       <c r="F712" s="9" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="G712" s="9" t="s">
         <v>10</v>
@@ -16309,27 +16309,27 @@
       <c r="H712" s="9"/>
       <c r="I712" s="9"/>
       <c r="J712" s="7" t="s">
-        <v>117</v>
+        <v>281</v>
       </c>
       <c r="K712" s="7" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
     </row>
     <row r="713" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B713" s="7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C713" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D713" s="17" t="s">
-        <v>375</v>
+        <v>174</v>
+      </c>
+      <c r="D713" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="E713" s="9" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F713" s="9" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
       <c r="G713" s="9" t="s">
         <v>10</v>
@@ -16337,10 +16337,10 @@
       <c r="H713" s="9"/>
       <c r="I713" s="9"/>
       <c r="J713" s="7" t="s">
-        <v>181</v>
+        <v>554</v>
       </c>
       <c r="K713" s="7" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
     </row>
     <row r="714" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16360,34 +16360,34 @@
       <c r="N714" s="1"/>
       <c r="O714" s="1"/>
     </row>
-    <row r="715" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A715" s="7" t="s">
+    <row r="715" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A715" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B715" s="7" t="s">
-        <v>486</v>
-      </c>
-      <c r="C715" s="7" t="s">
-        <v>487</v>
-      </c>
-      <c r="D715" s="7" t="s">
-        <v>488</v>
-      </c>
-      <c r="E715" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F715" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G715" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H715" s="9"/>
-      <c r="I715" s="9"/>
-      <c r="J715" s="7" t="s">
-        <v>489</v>
-      </c>
-      <c r="K715" s="7" t="s">
+      <c r="B715" s="13" t="s">
+        <v>576</v>
+      </c>
+      <c r="C715" s="13" t="s">
+        <v>577</v>
+      </c>
+      <c r="D715" s="13" t="s">
+        <v>578</v>
+      </c>
+      <c r="E715" s="14" t="s">
+        <v>579</v>
+      </c>
+      <c r="F715" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G715" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H715" s="14"/>
+      <c r="I715" s="14"/>
+      <c r="J715" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="K715" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -21282,16 +21282,16 @@
         <v>5</v>
       </c>
       <c r="B984" s="13" t="s">
-        <v>559</v>
+        <v>576</v>
       </c>
       <c r="C984" s="13" t="s">
-        <v>560</v>
+        <v>577</v>
       </c>
       <c r="D984" s="13" t="s">
-        <v>561</v>
+        <v>578</v>
       </c>
       <c r="E984" s="14" t="s">
-        <v>562</v>
+        <v>579</v>
       </c>
       <c r="F984" s="14" t="s">
         <v>41</v>
@@ -21304,7 +21304,7 @@
       </c>
       <c r="I984" s="14"/>
       <c r="J984" s="13" t="s">
-        <v>563</v>
+        <v>580</v>
       </c>
       <c r="K984" s="13" t="s">
         <v>43</v>
@@ -22529,16 +22529,16 @@
     </row>
     <row r="1041" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1041" s="13" t="s">
-        <v>559</v>
+        <v>576</v>
       </c>
       <c r="C1041" s="13" t="s">
-        <v>560</v>
+        <v>577</v>
       </c>
       <c r="D1041" s="13" t="s">
-        <v>561</v>
+        <v>578</v>
       </c>
       <c r="E1041" s="14" t="s">
-        <v>562</v>
+        <v>579</v>
       </c>
       <c r="F1041" s="14" t="s">
         <v>41</v>
@@ -22549,7 +22549,7 @@
       <c r="H1041" s="14"/>
       <c r="I1041" s="14"/>
       <c r="J1041" s="13" t="s">
-        <v>563</v>
+        <v>580</v>
       </c>
       <c r="K1041" s="13" t="s">
         <v>43</v>
@@ -22605,7 +22605,7 @@
       <c r="H1043" s="14"/>
       <c r="I1043" s="14"/>
       <c r="J1043" s="13" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="K1043" s="13" t="s">
         <v>43</v>
@@ -41181,16 +41181,16 @@
     </row>
     <row r="1148" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1148" s="13" t="s">
-        <v>559</v>
+        <v>576</v>
       </c>
       <c r="C1148" s="13" t="s">
-        <v>560</v>
+        <v>577</v>
       </c>
       <c r="D1148" s="13" t="s">
-        <v>561</v>
+        <v>578</v>
       </c>
       <c r="E1148" s="14" t="s">
-        <v>562</v>
+        <v>579</v>
       </c>
       <c r="F1148" s="14" t="s">
         <v>41</v>
@@ -41201,7 +41201,7 @@
       <c r="H1148" s="14"/>
       <c r="I1148" s="14"/>
       <c r="J1148" s="13" t="s">
-        <v>563</v>
+        <v>580</v>
       </c>
       <c r="K1148" s="13" t="s">
         <v>43</v>
@@ -41369,7 +41369,7 @@
       <c r="H1154" s="14"/>
       <c r="I1154" s="14"/>
       <c r="J1154" s="13" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="K1154" s="13" t="s">
         <v>43</v>
@@ -41682,16 +41682,16 @@
     </row>
     <row r="1166" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1166" s="7" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="C1166" s="7" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="D1166" s="7" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="E1166" s="9" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="F1166" s="9" t="s">
         <v>256</v>
@@ -41736,6 +41736,7 @@
         <v>43</v>
       </c>
     </row>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>